<commit_message>
Burdown update, Sql for Product added
</commit_message>
<xml_diff>
--- a/Docs/BurnDown.xlsx
+++ b/Docs/BurnDown.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\haral\Documents\GitHub\H1PD021123_Grp1_ERP\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B53C2A3-ADC3-4ED0-8611-D7DE4A0DE55A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B9DE0F0-94A0-47D7-9211-A6814DC2E8C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D641E094-DAC4-49DC-BC8B-5218FA1821D9}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="88">
   <si>
     <t>Date</t>
   </si>
@@ -300,6 +300,9 @@
   </si>
   <si>
     <t>har - 28/3</t>
+  </si>
+  <si>
+    <t>Har - 29/3</t>
   </si>
 </sst>
 </file>
@@ -5381,7 +5384,7 @@
   <dimension ref="A1:AK195"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" zoomScale="81" workbookViewId="0">
-      <selection activeCell="C42" sqref="C42"/>
+      <selection activeCell="F40" sqref="F40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6989,7 +6992,7 @@
         <v>83</v>
       </c>
       <c r="I36" s="60" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="J36" s="61" t="s">
         <v>80</v>

</xml_diff>

<commit_message>
[S2, S3] - 2.5 - Databases changes
</commit_message>
<xml_diff>
--- a/Docs/BurnDown.xlsx
+++ b/Docs/BurnDown.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\haral\Documents\GitHub\H1PD021123_Grp1_ERP\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC78BED1-0934-4BDB-9DE7-310721F1B3CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16438103-EC04-4E52-9C4F-74DD543A25E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D641E094-DAC4-49DC-BC8B-5218FA1821D9}"/>
+    <workbookView xWindow="1350" yWindow="-15870" windowWidth="25440" windowHeight="15390" xr2:uid="{D641E094-DAC4-49DC-BC8B-5218FA1821D9}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="91">
   <si>
     <t>Date</t>
   </si>
@@ -303,6 +303,15 @@
   </si>
   <si>
     <t>Har - 30/3</t>
+  </si>
+  <si>
+    <t>Mar - 12/4</t>
+  </si>
+  <si>
+    <t>Nic - 12/4</t>
+  </si>
+  <si>
+    <t>Nic -12/4</t>
   </si>
 </sst>
 </file>
@@ -5384,7 +5393,7 @@
   <dimension ref="A1:AK195"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A18" zoomScale="81" workbookViewId="0">
-      <selection activeCell="H40" sqref="H40"/>
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7027,9 +7036,7 @@
     </row>
     <row r="37" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A37" s="45"/>
-      <c r="B37" s="18" t="s">
-        <v>34</v>
-      </c>
+      <c r="B37" s="18"/>
       <c r="C37" s="12"/>
       <c r="D37" s="15"/>
       <c r="E37" s="52" t="s">
@@ -7044,8 +7051,12 @@
       <c r="H37" s="62" t="s">
         <v>36</v>
       </c>
-      <c r="I37" s="63"/>
-      <c r="J37" s="64"/>
+      <c r="I37" s="63" t="s">
+        <v>33</v>
+      </c>
+      <c r="J37" s="64" t="s">
+        <v>34</v>
+      </c>
       <c r="K37" s="45"/>
       <c r="L37" s="45"/>
       <c r="M37" s="45"/>
@@ -7091,8 +7102,12 @@
       <c r="H38" s="59" t="s">
         <v>87</v>
       </c>
-      <c r="I38" s="60"/>
-      <c r="J38" s="61"/>
+      <c r="I38" s="60" t="s">
+        <v>88</v>
+      </c>
+      <c r="J38" s="61" t="s">
+        <v>88</v>
+      </c>
       <c r="K38" s="45"/>
       <c r="L38" s="88" t="s">
         <v>77</v>
@@ -7126,19 +7141,23 @@
     <row r="39" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A39" s="45"/>
       <c r="B39" s="18"/>
-      <c r="C39" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="D39" s="15" t="s">
-        <v>13</v>
-      </c>
+      <c r="C39" s="12"/>
+      <c r="D39" s="15"/>
       <c r="E39" s="52" t="s">
         <v>36</v>
       </c>
-      <c r="F39" s="47"/>
-      <c r="G39" s="48"/>
-      <c r="H39" s="62"/>
-      <c r="I39" s="63"/>
+      <c r="F39" s="47" t="s">
+        <v>34</v>
+      </c>
+      <c r="G39" s="48" t="s">
+        <v>38</v>
+      </c>
+      <c r="H39" s="62" t="s">
+        <v>31</v>
+      </c>
+      <c r="I39" s="63" t="s">
+        <v>37</v>
+      </c>
       <c r="J39" s="64"/>
       <c r="K39" s="45"/>
       <c r="L39" s="4" t="s">
@@ -7182,10 +7201,18 @@
       <c r="E40" s="49" t="s">
         <v>85</v>
       </c>
-      <c r="F40" s="50"/>
-      <c r="G40" s="51"/>
-      <c r="H40" s="59"/>
-      <c r="I40" s="60"/>
+      <c r="F40" s="50" t="s">
+        <v>88</v>
+      </c>
+      <c r="G40" s="51" t="s">
+        <v>90</v>
+      </c>
+      <c r="H40" s="59" t="s">
+        <v>88</v>
+      </c>
+      <c r="I40" s="60" t="s">
+        <v>89</v>
+      </c>
       <c r="J40" s="61"/>
       <c r="K40" s="45"/>
       <c r="L40" s="88">
@@ -7223,7 +7250,9 @@
       <c r="B41" s="18"/>
       <c r="C41" s="12"/>
       <c r="D41" s="15"/>
-      <c r="E41" s="52"/>
+      <c r="E41" s="52" t="s">
+        <v>13</v>
+      </c>
       <c r="F41" s="47"/>
       <c r="G41" s="48"/>
       <c r="H41" s="62"/>
@@ -7265,7 +7294,9 @@
       <c r="B42" s="16"/>
       <c r="C42" s="14"/>
       <c r="D42" s="17"/>
-      <c r="E42" s="49"/>
+      <c r="E42" s="49" t="s">
+        <v>89</v>
+      </c>
       <c r="F42" s="50"/>
       <c r="G42" s="51"/>
       <c r="H42" s="59"/>

</xml_diff>

<commit_message>
[S2, S3] - 2.7 - Insert to work with new Database
</commit_message>
<xml_diff>
--- a/Docs/BurnDown.xlsx
+++ b/Docs/BurnDown.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\haral\Documents\GitHub\H1PD021123_Grp1_ERP\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16438103-EC04-4E52-9C4F-74DD543A25E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0F9B791-09D4-4740-8E5A-251DEE059A38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1350" yWindow="-15870" windowWidth="25440" windowHeight="15390" xr2:uid="{D641E094-DAC4-49DC-BC8B-5218FA1821D9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D641E094-DAC4-49DC-BC8B-5218FA1821D9}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="91">
   <si>
     <t>Date</t>
   </si>
@@ -1642,6 +1642,9 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -5392,8 +5395,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF0B712E-09C2-44DE-B884-3CC21268FBEE}">
   <dimension ref="A1:AK195"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="81" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="81" workbookViewId="0">
+      <selection activeCell="I44" sqref="I44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6946,9 +6949,7 @@
       <c r="G35" s="48" t="s">
         <v>37</v>
       </c>
-      <c r="H35" s="56" t="s">
-        <v>31</v>
-      </c>
+      <c r="H35" s="56"/>
       <c r="I35" s="57" t="s">
         <v>84</v>
       </c>
@@ -6997,9 +6998,7 @@
       <c r="G36" s="51" t="s">
         <v>82</v>
       </c>
-      <c r="H36" s="59" t="s">
-        <v>83</v>
-      </c>
+      <c r="H36" s="59"/>
       <c r="I36" s="60" t="s">
         <v>86</v>
       </c>
@@ -7220,6 +7219,9 @@
       </c>
       <c r="M40" s="4">
         <v>7</v>
+      </c>
+      <c r="N40" s="4">
+        <v>3</v>
       </c>
       <c r="O40" s="45"/>
       <c r="P40" s="45"/>

</xml_diff>

<commit_message>
Bug fixing - not displaying data
</commit_message>
<xml_diff>
--- a/Docs/BurnDown.xlsx
+++ b/Docs/BurnDown.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\haral\Documents\GitHub\H1PD021123_Grp1_ERP\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC78BED1-0934-4BDB-9DE7-310721F1B3CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0F9B791-09D4-4740-8E5A-251DEE059A38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D641E094-DAC4-49DC-BC8B-5218FA1821D9}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="91">
   <si>
     <t>Date</t>
   </si>
@@ -303,6 +303,15 @@
   </si>
   <si>
     <t>Har - 30/3</t>
+  </si>
+  <si>
+    <t>Mar - 12/4</t>
+  </si>
+  <si>
+    <t>Nic - 12/4</t>
+  </si>
+  <si>
+    <t>Nic -12/4</t>
   </si>
 </sst>
 </file>
@@ -1633,6 +1642,9 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -5383,8 +5395,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF0B712E-09C2-44DE-B884-3CC21268FBEE}">
   <dimension ref="A1:AK195"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="81" workbookViewId="0">
-      <selection activeCell="H40" sqref="H40"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="81" workbookViewId="0">
+      <selection activeCell="I44" sqref="I44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6937,9 +6949,7 @@
       <c r="G35" s="48" t="s">
         <v>37</v>
       </c>
-      <c r="H35" s="56" t="s">
-        <v>31</v>
-      </c>
+      <c r="H35" s="56"/>
       <c r="I35" s="57" t="s">
         <v>84</v>
       </c>
@@ -6988,9 +6998,7 @@
       <c r="G36" s="51" t="s">
         <v>82</v>
       </c>
-      <c r="H36" s="59" t="s">
-        <v>83</v>
-      </c>
+      <c r="H36" s="59"/>
       <c r="I36" s="60" t="s">
         <v>86</v>
       </c>
@@ -7027,9 +7035,7 @@
     </row>
     <row r="37" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A37" s="45"/>
-      <c r="B37" s="18" t="s">
-        <v>34</v>
-      </c>
+      <c r="B37" s="18"/>
       <c r="C37" s="12"/>
       <c r="D37" s="15"/>
       <c r="E37" s="52" t="s">
@@ -7044,8 +7050,12 @@
       <c r="H37" s="62" t="s">
         <v>36</v>
       </c>
-      <c r="I37" s="63"/>
-      <c r="J37" s="64"/>
+      <c r="I37" s="63" t="s">
+        <v>33</v>
+      </c>
+      <c r="J37" s="64" t="s">
+        <v>34</v>
+      </c>
       <c r="K37" s="45"/>
       <c r="L37" s="45"/>
       <c r="M37" s="45"/>
@@ -7091,8 +7101,12 @@
       <c r="H38" s="59" t="s">
         <v>87</v>
       </c>
-      <c r="I38" s="60"/>
-      <c r="J38" s="61"/>
+      <c r="I38" s="60" t="s">
+        <v>88</v>
+      </c>
+      <c r="J38" s="61" t="s">
+        <v>88</v>
+      </c>
       <c r="K38" s="45"/>
       <c r="L38" s="88" t="s">
         <v>77</v>
@@ -7126,19 +7140,23 @@
     <row r="39" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A39" s="45"/>
       <c r="B39" s="18"/>
-      <c r="C39" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="D39" s="15" t="s">
-        <v>13</v>
-      </c>
+      <c r="C39" s="12"/>
+      <c r="D39" s="15"/>
       <c r="E39" s="52" t="s">
         <v>36</v>
       </c>
-      <c r="F39" s="47"/>
-      <c r="G39" s="48"/>
-      <c r="H39" s="62"/>
-      <c r="I39" s="63"/>
+      <c r="F39" s="47" t="s">
+        <v>34</v>
+      </c>
+      <c r="G39" s="48" t="s">
+        <v>38</v>
+      </c>
+      <c r="H39" s="62" t="s">
+        <v>31</v>
+      </c>
+      <c r="I39" s="63" t="s">
+        <v>37</v>
+      </c>
       <c r="J39" s="64"/>
       <c r="K39" s="45"/>
       <c r="L39" s="4" t="s">
@@ -7182,10 +7200,18 @@
       <c r="E40" s="49" t="s">
         <v>85</v>
       </c>
-      <c r="F40" s="50"/>
-      <c r="G40" s="51"/>
-      <c r="H40" s="59"/>
-      <c r="I40" s="60"/>
+      <c r="F40" s="50" t="s">
+        <v>88</v>
+      </c>
+      <c r="G40" s="51" t="s">
+        <v>90</v>
+      </c>
+      <c r="H40" s="59" t="s">
+        <v>88</v>
+      </c>
+      <c r="I40" s="60" t="s">
+        <v>89</v>
+      </c>
       <c r="J40" s="61"/>
       <c r="K40" s="45"/>
       <c r="L40" s="88">
@@ -7193,6 +7219,9 @@
       </c>
       <c r="M40" s="4">
         <v>7</v>
+      </c>
+      <c r="N40" s="4">
+        <v>3</v>
       </c>
       <c r="O40" s="45"/>
       <c r="P40" s="45"/>
@@ -7223,7 +7252,9 @@
       <c r="B41" s="18"/>
       <c r="C41" s="12"/>
       <c r="D41" s="15"/>
-      <c r="E41" s="52"/>
+      <c r="E41" s="52" t="s">
+        <v>13</v>
+      </c>
       <c r="F41" s="47"/>
       <c r="G41" s="48"/>
       <c r="H41" s="62"/>
@@ -7265,7 +7296,9 @@
       <c r="B42" s="16"/>
       <c r="C42" s="14"/>
       <c r="D42" s="17"/>
-      <c r="E42" s="49"/>
+      <c r="E42" s="49" t="s">
+        <v>89</v>
+      </c>
       <c r="F42" s="50"/>
       <c r="G42" s="51"/>
       <c r="H42" s="59"/>

</xml_diff>